<commit_message>
fix: inversion sole and prey contam (another time !)
</commit_message>
<xml_diff>
--- a/inst/results/BMF_computation_PFAS_ng_gdw/3.BMF_diet_PFAS_ng_gdw_uncensored.xlsx
+++ b/inst/results/BMF_computation_PFAS_ng_gdw/3.BMF_diet_PFAS_ng_gdw_uncensored.xlsx
@@ -416,31 +416,31 @@
         </is>
       </c>
       <c r="B2">
+        <v>0.01</v>
+      </c>
+      <c r="C2">
+        <v>0.01</v>
+      </c>
+      <c r="D2">
+        <v>0.13</v>
+      </c>
+      <c r="E2">
         <v>0.05</v>
       </c>
-      <c r="C2">
+      <c r="F2">
         <v>0.1</v>
       </c>
-      <c r="D2">
+      <c r="G2">
         <v>0.2</v>
       </c>
-      <c r="E2">
-        <v>0.01</v>
-      </c>
-      <c r="F2">
-        <v>0.01</v>
-      </c>
-      <c r="G2">
-        <v>0.13</v>
-      </c>
       <c r="H2">
-        <v>0.36</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I2">
-        <v>6.51</v>
+        <v>0.15</v>
       </c>
       <c r="J2">
-        <v>13.8</v>
+        <v>2.82</v>
       </c>
     </row>
     <row r="3">
@@ -450,31 +450,31 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.35</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="C3">
+        <v>1.41</v>
+      </c>
+      <c r="D3">
+        <v>2.79</v>
+      </c>
+      <c r="E3">
+        <v>0.38</v>
+      </c>
+      <c r="F3">
         <v>0.5600000000000001</v>
       </c>
-      <c r="D3">
+      <c r="G3">
         <v>0.92</v>
       </c>
-      <c r="E3">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="F3">
-        <v>1.41</v>
-      </c>
-      <c r="G3">
-        <v>2.79</v>
-      </c>
       <c r="H3">
-        <v>0.13</v>
+        <v>1.03</v>
       </c>
       <c r="I3">
-        <v>0.4</v>
+        <v>2.54</v>
       </c>
       <c r="J3">
-        <v>0.97</v>
+        <v>7.33</v>
       </c>
     </row>
     <row r="4">
@@ -484,31 +484,31 @@
         </is>
       </c>
       <c r="B4">
+        <v>0.12</v>
+      </c>
+      <c r="C4">
+        <v>0.22</v>
+      </c>
+      <c r="D4">
+        <v>0.37</v>
+      </c>
+      <c r="E4">
         <v>0.23</v>
       </c>
-      <c r="C4">
+      <c r="F4">
         <v>0.37</v>
       </c>
-      <c r="D4">
+      <c r="G4">
         <v>0.8100000000000001</v>
       </c>
-      <c r="E4">
-        <v>0.12</v>
-      </c>
-      <c r="F4">
-        <v>0.22</v>
-      </c>
-      <c r="G4">
-        <v>0.37</v>
-      </c>
       <c r="H4">
-        <v>0.61</v>
+        <v>0.15</v>
       </c>
       <c r="I4">
+        <v>0.6</v>
+      </c>
+      <c r="J4">
         <v>1.66</v>
-      </c>
-      <c r="J4">
-        <v>6.63</v>
       </c>
     </row>
     <row r="5">
@@ -518,31 +518,31 @@
         </is>
       </c>
       <c r="B5">
+        <v>0.24</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>0.92</v>
+      </c>
+      <c r="E5">
         <v>2.07</v>
       </c>
-      <c r="C5">
+      <c r="F5">
         <v>2.51</v>
       </c>
-      <c r="D5">
+      <c r="G5">
         <v>3.93</v>
       </c>
-      <c r="E5">
-        <v>0.24</v>
-      </c>
-      <c r="F5">
-        <v>0.5</v>
-      </c>
-      <c r="G5">
-        <v>0.92</v>
-      </c>
       <c r="H5">
-        <v>2.24</v>
+        <v>0.06</v>
       </c>
       <c r="I5">
-        <v>5.03</v>
+        <v>0.2</v>
       </c>
       <c r="J5">
-        <v>16.37</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="6">
@@ -552,31 +552,31 @@
         </is>
       </c>
       <c r="B6">
+        <v>8.91</v>
+      </c>
+      <c r="C6">
+        <v>10.59</v>
+      </c>
+      <c r="D6">
+        <v>13.75</v>
+      </c>
+      <c r="E6">
         <v>4.63</v>
       </c>
-      <c r="C6">
+      <c r="F6">
         <v>6.74</v>
       </c>
-      <c r="D6">
+      <c r="G6">
         <v>9.720000000000001</v>
       </c>
-      <c r="E6">
-        <v>8.91</v>
-      </c>
-      <c r="F6">
-        <v>10.59</v>
-      </c>
-      <c r="G6">
-        <v>13.75</v>
-      </c>
       <c r="H6">
-        <v>0.34</v>
+        <v>0.92</v>
       </c>
       <c r="I6">
-        <v>0.64</v>
+        <v>1.57</v>
       </c>
       <c r="J6">
-        <v>1.09</v>
+        <v>2.97</v>
       </c>
     </row>
     <row r="7">
@@ -586,31 +586,31 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.48</v>
+        <v>1.1</v>
       </c>
       <c r="C7">
+        <v>1.57</v>
+      </c>
+      <c r="D7">
+        <v>2.15</v>
+      </c>
+      <c r="E7">
+        <v>0.46</v>
+      </c>
+      <c r="F7">
         <v>1.03</v>
       </c>
-      <c r="D7">
+      <c r="G7">
         <v>1.3</v>
       </c>
-      <c r="E7">
-        <v>1.1</v>
-      </c>
-      <c r="F7">
-        <v>1.57</v>
-      </c>
-      <c r="G7">
-        <v>2.15</v>
-      </c>
       <c r="H7">
-        <v>0.22</v>
+        <v>0.84</v>
       </c>
       <c r="I7">
-        <v>0.66</v>
+        <v>1.52</v>
       </c>
       <c r="J7">
-        <v>1.19</v>
+        <v>4.65</v>
       </c>
     </row>
     <row r="8">
@@ -620,31 +620,31 @@
         </is>
       </c>
       <c r="B8">
+        <v>0.66</v>
+      </c>
+      <c r="C8">
+        <v>1.01</v>
+      </c>
+      <c r="D8">
+        <v>1.24</v>
+      </c>
+      <c r="E8">
         <v>0.55</v>
       </c>
-      <c r="C8">
+      <c r="F8">
         <v>0.72</v>
       </c>
-      <c r="D8">
+      <c r="G8">
         <v>0.97</v>
       </c>
-      <c r="E8">
-        <v>0.66</v>
-      </c>
-      <c r="F8">
-        <v>1.01</v>
-      </c>
-      <c r="G8">
-        <v>1.24</v>
-      </c>
       <c r="H8">
-        <v>0.45</v>
+        <v>0.68</v>
       </c>
       <c r="I8">
-        <v>0.71</v>
+        <v>1.4</v>
       </c>
       <c r="J8">
-        <v>1.47</v>
+        <v>2.24</v>
       </c>
     </row>
     <row r="9">
@@ -654,31 +654,31 @@
         </is>
       </c>
       <c r="B9">
+        <v>0.89</v>
+      </c>
+      <c r="C9">
+        <v>1.14</v>
+      </c>
+      <c r="D9">
+        <v>1.8</v>
+      </c>
+      <c r="E9">
         <v>0.42</v>
       </c>
-      <c r="C9">
+      <c r="F9">
         <v>0.5600000000000001</v>
       </c>
-      <c r="D9">
+      <c r="G9">
         <v>0.89</v>
       </c>
-      <c r="E9">
-        <v>0.89</v>
-      </c>
-      <c r="F9">
-        <v>1.14</v>
-      </c>
-      <c r="G9">
-        <v>1.8</v>
-      </c>
       <c r="H9">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>0.49</v>
+        <v>2.03</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>4.31</v>
       </c>
     </row>
     <row r="10">
@@ -691,28 +691,28 @@
         <v>0.02</v>
       </c>
       <c r="C10">
-        <v>0.48</v>
+        <v>0.02</v>
       </c>
       <c r="D10">
-        <v>0.88</v>
+        <v>0.63</v>
       </c>
       <c r="E10">
         <v>0.02</v>
       </c>
       <c r="F10">
-        <v>0.02</v>
+        <v>0.48</v>
       </c>
       <c r="G10">
-        <v>0.63</v>
+        <v>0.88</v>
       </c>
       <c r="H10">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I10">
-        <v>19.45</v>
+        <v>0.05</v>
       </c>
       <c r="J10">
-        <v>40.28</v>
+        <v>26.3</v>
       </c>
     </row>
     <row r="11">
@@ -722,31 +722,31 @@
         </is>
       </c>
       <c r="B11">
+        <v>0.24</v>
+      </c>
+      <c r="C11">
+        <v>0.41</v>
+      </c>
+      <c r="D11">
+        <v>0.45</v>
+      </c>
+      <c r="E11">
         <v>0.13</v>
       </c>
-      <c r="C11">
+      <c r="F11">
         <v>0.18</v>
       </c>
-      <c r="D11">
+      <c r="G11">
         <v>0.28</v>
       </c>
-      <c r="E11">
-        <v>0.24</v>
-      </c>
-      <c r="F11">
-        <v>0.41</v>
-      </c>
-      <c r="G11">
-        <v>0.45</v>
-      </c>
       <c r="H11">
-        <v>0.3</v>
+        <v>0.84</v>
       </c>
       <c r="I11">
-        <v>0.44</v>
+        <v>2.28</v>
       </c>
       <c r="J11">
-        <v>1.19</v>
+        <v>3.35</v>
       </c>
     </row>
     <row r="12">
@@ -756,31 +756,31 @@
         </is>
       </c>
       <c r="B12">
+        <v>0.08</v>
+      </c>
+      <c r="C12">
+        <v>0.08</v>
+      </c>
+      <c r="D12">
+        <v>0.23</v>
+      </c>
+      <c r="E12">
         <v>0.15</v>
       </c>
-      <c r="C12">
+      <c r="F12">
         <v>0.24</v>
       </c>
-      <c r="D12">
+      <c r="G12">
         <v>0.37</v>
       </c>
-      <c r="E12">
-        <v>0.08</v>
-      </c>
-      <c r="F12">
-        <v>0.08</v>
-      </c>
-      <c r="G12">
-        <v>0.23</v>
-      </c>
       <c r="H12">
-        <v>0.66</v>
+        <v>0.21</v>
       </c>
       <c r="I12">
-        <v>2.95</v>
+        <v>0.35</v>
       </c>
       <c r="J12">
-        <v>4.61</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="13">
@@ -790,31 +790,31 @@
         </is>
       </c>
       <c r="B13">
-        <v>10.86</v>
+        <v>14.32</v>
       </c>
       <c r="C13">
-        <v>15.41</v>
+        <v>17.16</v>
       </c>
       <c r="D13">
-        <v>18.94</v>
+        <v>25.8</v>
       </c>
       <c r="E13">
-        <v>14.32</v>
+        <v>10.88</v>
       </c>
       <c r="F13">
-        <v>17.19</v>
+        <v>15.45</v>
       </c>
       <c r="G13">
-        <v>25.8</v>
+        <v>18.95</v>
       </c>
       <c r="H13">
-        <v>0.42</v>
+        <v>0.76</v>
       </c>
       <c r="I13">
-        <v>0.9</v>
+        <v>1.11</v>
       </c>
       <c r="J13">
-        <v>1.32</v>
+        <v>2.37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>